<commit_message>
New data and plots added
</commit_message>
<xml_diff>
--- a/Data/newdata/Materials/QR-13AF_data.xlsx
+++ b/Data/newdata/Materials/QR-13AF_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\UMKC Physics Research 16\MATERIALS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jl3y9\Documents\MATLAB\Data\newdata\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="8868"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,13 +338,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0.5</v>
       </c>
@@ -355,13 +355,13 @@
         <v>27.887271303670499</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.75</v>
       </c>
@@ -372,13 +372,13 @@
         <v>25.855952501685</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -389,13 +389,13 @@
         <v>23.929235967243901</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.25</v>
       </c>
@@ -406,13 +406,13 @@
         <v>21.9391727476022</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -423,13 +423,13 @@
         <v>19.998197548888101</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.75</v>
       </c>
@@ -440,13 +440,13 @@
         <v>18.717796708858501</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -457,13 +457,13 @@
         <v>17.426002174328499</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2.25</v>
       </c>
@@ -474,13 +474,13 @@
         <v>16.207392452255</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2.5</v>
       </c>
@@ -491,13 +491,13 @@
         <v>15.0003317668561</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2.75</v>
       </c>
@@ -508,13 +508,13 @@
         <v>14.2140899684358</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -525,13 +525,13 @@
         <v>13.4937027625783</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.25</v>
       </c>
@@ -542,13 +542,13 @@
         <v>12.702341011098699</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3.5</v>
       </c>
@@ -559,13 +559,13 @@
         <v>11.901059408130701</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3.75</v>
       </c>
@@ -576,13 +576,13 @@
         <v>11.3527672279325</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -593,13 +593,13 @@
         <v>10.8746499742123</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4.25</v>
       </c>
@@ -610,13 +610,13 @@
         <v>10.3306815385784</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4.5</v>
       </c>
@@ -627,13 +627,13 @@
         <v>9.9194941979159807</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4.75</v>
       </c>
@@ -644,13 +644,13 @@
         <v>9.4083701497270695</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -661,13 +661,13 @@
         <v>8.8352088778709508</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5.25</v>
       </c>
@@ -678,13 +678,13 @@
         <v>8.4175400059219392</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5.5</v>
       </c>
@@ -695,13 +695,13 @@
         <v>8.0051726945353199</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5.75</v>
       </c>
@@ -712,13 +712,13 @@
         <v>7.7277156918031604</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -729,13 +729,13 @@
         <v>7.7284120349017904</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6.25</v>
       </c>
@@ -746,13 +746,13 @@
         <v>7.5020891097777804</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6.5</v>
       </c>
@@ -763,13 +763,13 @@
         <v>7.5030190920958901</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6.75</v>
       </c>
@@ -780,13 +780,13 @@
         <v>7.2764620380079199</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -797,13 +797,13 @@
         <v>7.2198977484764102</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7.25</v>
       </c>
@@ -814,13 +814,13 @@
         <v>6.9381195059035798</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7.5</v>
       </c>
@@ -831,13 +831,13 @@
         <v>6.9435562768801899</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7.75</v>
       </c>
@@ -848,13 +848,13 @@
         <v>6.7123955681699004</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -865,13 +865,13 @@
         <v>6.7126768524404596</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8.25</v>
       </c>
@@ -882,13 +882,13 @@
         <v>6.4867695794771398</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8.5</v>
       </c>
@@ -899,13 +899,13 @@
         <v>6.4865556207814103</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8.75</v>
       </c>
@@ -916,13 +916,13 @@
         <v>6.26104023120687</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9</v>
       </c>
@@ -933,13 +933,13 @@
         <v>6.1483262569600896</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>9.25</v>
       </c>
@@ -950,13 +950,13 @@
         <v>5.9226790003035701</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9.5</v>
       </c>
@@ -967,13 +967,13 @@
         <v>5.9227052440123904</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>9.75</v>
       </c>
@@ -984,13 +984,13 @@
         <v>5.6970829806202001</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10</v>
       </c>
@@ -1001,13 +1001,13 @@
         <v>5.6970771797111501</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10.25</v>
       </c>
@@ -1018,13 +1018,13 @@
         <v>5.4713965041610404</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10.5</v>
       </c>
@@ -1035,13 +1035,13 @@
         <v>5.4716581085885103</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10.75</v>
       </c>
@@ -1052,13 +1052,13 @@
         <v>5.1294033977190798</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
@@ -1069,13 +1069,13 @@
         <v>5.0203735174550204</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>11.25</v>
       </c>
@@ -1086,13 +1086,13 @@
         <v>4.9032702756190503</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>11.5</v>
       </c>
@@ -1103,13 +1103,13 @@
         <v>4.9073816114346904</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>11.75</v>
       </c>
@@ -1120,13 +1120,13 @@
         <v>4.6772046105242699</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>12</v>
       </c>
@@ -1137,13 +1137,13 @@
         <v>4.6817548868562797</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>12.25</v>
       </c>
@@ -1154,13 +1154,13 @@
         <v>4.4999375706217899</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>12.5</v>
       </c>
@@ -1171,13 +1171,13 @@
         <v>4.5130722630989197</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>12.75</v>
       </c>
@@ -1188,13 +1188,13 @@
         <v>4.3216117529212097</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>13</v>
       </c>
@@ -1205,13 +1205,13 @@
         <v>4.1176880445948303</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>13.25</v>
       </c>
@@ -1222,13 +1222,13 @@
         <v>3.8963516026337301</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>13.5</v>
       </c>
@@ -1239,13 +1239,13 @@
         <v>3.89206128172443</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>13.75</v>
       </c>
@@ -1256,13 +1256,13 @@
         <v>3.8920612813369502</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>14</v>
       </c>
@@ -1273,13 +1273,13 @@
         <v>3.8920639853074399</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>14.25</v>
       </c>
@@ -1290,13 +1290,13 @@
         <v>3.6694292075869801</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14.5</v>
       </c>
@@ -1307,13 +1307,13 @@
         <v>3.6664345404113998</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>14.75</v>
       </c>
@@ -1324,13 +1324,13 @@
         <v>3.66643638767966</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>15</v>
       </c>
@@ -1341,13 +1341,13 @@
         <v>3.5552787249773901</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15.249999999999901</v>
       </c>
@@ -1358,13 +1358,13 @@
         <v>3.3280414013451098</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15.499999999999901</v>
       </c>
@@ -1375,13 +1375,13 @@
         <v>3.32799442896671</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15.749999999999901</v>
       </c>
@@ -1392,13 +1392,13 @@
         <v>3.32799442896978</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>15.999999999999901</v>
       </c>
@@ -1409,13 +1409,13 @@
         <v>3.3279938786410899</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>16.25</v>
       </c>
@@ -1426,13 +1426,13 @@
         <v>3.1017315029678501</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>16.5</v>
       </c>
@@ -1443,13 +1443,13 @@
         <v>3.1023676880142399</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>16.75</v>
       </c>
@@ -1460,13 +1460,13 @@
         <v>3.1023676880222002</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>17</v>
       </c>
@@ -1477,13 +1477,13 @@
         <v>3.1023515392075498</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>17.25</v>
       </c>
@@ -1494,10 +1494,10 @@
         <v>2.8766919895681999</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>